<commit_message>
Closed out sprint 5, started sprint 6
</commit_message>
<xml_diff>
--- a/project/Sprint05.xlsx
+++ b/project/Sprint05.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmiele\Documents\Masters\CSE551\CSE551\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Documents\masters\cse551\CSE551\project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -134,7 +134,8 @@
     <t>Read and note paper</t>
   </si>
   <si>
-    <t>HW2 ate a lot of the last iteration. Going to try to focus on getting a draft of the paper done.</t>
+    <t>HW2 ate a lot of the last iteration. Going to try to focus on getting a draft of the paper done.
+Got some work done on paper, plan to have initial draft done during next iteration</t>
   </si>
 </sst>
 </file>
@@ -528,10 +529,10 @@
                   <c:v>9.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.5</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.5</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1753,7 +1754,7 @@
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1820,36 +1821,36 @@
         <v>3</v>
       </c>
       <c r="D2" s="24">
-        <f>SUM(D$4:D$992)</f>
+        <f t="shared" ref="D2:K2" si="0">SUM(D$4:D$992)</f>
         <v>9.5</v>
       </c>
       <c r="E2" s="25">
-        <f>SUM(E$4:E$992)</f>
+        <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
       <c r="F2" s="25">
-        <f>SUM(F$4:F$992)</f>
+        <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
       <c r="G2" s="25">
-        <f>SUM(G$4:G$992)</f>
+        <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
       <c r="H2" s="25">
-        <f>SUM(H$4:H$992)</f>
+        <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
       <c r="I2" s="25">
-        <f>SUM(I$4:I$992)</f>
+        <f t="shared" si="0"/>
         <v>9.5</v>
       </c>
       <c r="J2" s="25">
-        <f>SUM(J$4:J$992)</f>
-        <v>9.5</v>
+        <f t="shared" si="0"/>
+        <v>6.5</v>
       </c>
       <c r="K2" s="25">
-        <f>SUM(K$4:K$992)</f>
-        <v>9.5</v>
+        <f t="shared" si="0"/>
+        <v>5.5</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1863,31 +1864,31 @@
         <v>9.5</v>
       </c>
       <c r="E3" s="25">
-        <f t="shared" ref="E3:K3" si="0">D$3-$D$2/7</f>
+        <f t="shared" ref="E3:K3" si="1">D$3-$D$2/7</f>
         <v>8.1428571428571423</v>
       </c>
       <c r="F3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.7857142857142847</v>
       </c>
       <c r="G3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.428571428571427</v>
       </c>
       <c r="H3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.0714285714285694</v>
       </c>
       <c r="I3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.7142857142857122</v>
       </c>
       <c r="J3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.357142857142855</v>
       </c>
       <c r="K3" s="25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.2204460492503131E-15</v>
       </c>
       <c r="L3" s="6" t="s">
@@ -1912,28 +1913,27 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <f t="shared" ref="F4:K4" si="1">E4</f>
+        <f t="shared" ref="F4:K4" si="2">E4</f>
         <v>2</v>
       </c>
       <c r="G4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J4">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <f t="shared" si="1"/>
-        <v>2</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -1957,32 +1957,31 @@
         <v>2</v>
       </c>
       <c r="E5">
-        <f t="shared" ref="E5:K10" si="2">D5</f>
+        <f t="shared" ref="E5:K10" si="3">D5</f>
         <v>2</v>
       </c>
       <c r="F5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="I5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="J5">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K5">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="L5" t="s">
         <v>27</v>
@@ -2006,32 +2005,31 @@
         <v>2</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="F6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="I6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="J6">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K6">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="L6" t="s">
         <v>26</v>
@@ -2055,31 +2053,31 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2097,31 +2095,31 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
@@ -2139,31 +2137,31 @@
         <v>0.5</v>
       </c>
       <c r="E9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="G9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="H9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="I9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="J9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="K9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
     </row>
@@ -2181,32 +2179,31 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="H10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="J10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="K10">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>